<commit_message>
02Dec2022 Created the consolidtion of SVC automaton
</commit_message>
<xml_diff>
--- a/Carg_Rediness/NDNL_/Out.xlsx
+++ b/Carg_Rediness/NDNL_/Out.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,52 +525,52 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SAINT JOHN, NB</t>
+          <t>HALIFAX, NS</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BALTIC FULMAR</t>
+          <t>MAERSK IDAHO</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BLFUL</t>
+          <t>MKIDO</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0UACZS1MA</t>
+          <t>0EDCME1MA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>CMA - CGM</t>
+          <t>MSK</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>9313204</v>
+        <v>9193264</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>44868.7916666551</v>
+        <v>44880.83333333334</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>44868.92916665509</v>
+        <v>44881.375</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>44869.375</v>
+        <v>44881.4166666551</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>44869.95833333334</v>
+        <v>44881.9166666551</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>CASJB</t>
+          <t>CAHAL</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -585,52 +585,52 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CHARLESTON</t>
+          <t>MIAMI</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MAERSK CHICAGO</t>
+          <t>GARFIELD</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MKCHG</t>
+          <t>GAFLD</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1JU16W1MA</t>
+          <t>0GY9EE1MA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>MSK</t>
+          <t>CMA - CGM</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9332975</v>
+        <v>9311842</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880.875</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>44869.33333333334</v>
+        <v>44882.0416666551</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>44869.5</v>
+        <v>44882.125</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>44869.9166666551</v>
+        <v>44882.6666666551</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>USCHS</t>
+          <t>USMIA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -645,22 +645,22 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CHARLESTON</t>
+          <t>NEW ORLEANS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CMA CGM MAGELLAN</t>
+          <t>CMA CGM VERACRUZ</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>CGMAG</t>
+          <t>CGVCZ</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0TUQ6N1MA</t>
+          <t>0GBDMS1MA</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -669,28 +669,28 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>9454424</v>
+        <v>9418377</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880.9166666551</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>44870.2916666551</v>
+        <v>44883.5416666551</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>44870.45833333334</v>
+        <v>44884.0416666551</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>44871.70833333334</v>
+        <v>44884.7916666551</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>USCHS</t>
+          <t>USMSY</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -705,52 +705,52 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HOUSTON</t>
+          <t>PORT HUENEME, CA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CMA CGM MUSSET</t>
+          <t>DEL MONTE HARVESTER</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CMMUS</t>
+          <t>DELHV</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0VBCIE1MA</t>
+          <t>0WS1LR1MA</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>CMA - CGM</t>
+          <t>DEL MONTE FRESH COMPANY</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>9406611</v>
+        <v>9869667</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>44868.9166666551</v>
+        <v>44880.83333333334</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>44862.47986111111</v>
+        <v>44883.34861111111</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>44871.45833333334</v>
+        <v>44883.3902777662</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>44873.0416666551</v>
+        <v>44884.93194444444</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>USHOU</t>
+          <t>USNTD</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -765,52 +765,52 @@
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LOS ANGELES, CA</t>
+          <t>NEW YORK</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>EVER ENVOY</t>
+          <t>NORTHERN PRIORITY</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EVENV</t>
+          <t>NTPRY</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0FTEGN1MA</t>
+          <t>0AMCFS1MA</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>EVERGREEN MARINE CORPORATION LTD</t>
+          <t>MSK</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>9241308</v>
+        <v>9450313</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>44868.95833333334</v>
+        <v>44880.875</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>44870.45833333334</v>
+        <v>44882.33333333334</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>44870.5416666551</v>
+        <v>44882.5</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>44873.125</v>
+        <v>44883.1666666551</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>USLAX</t>
+          <t>USNYC</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -825,52 +825,52 @@
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>LOS ANGELES, CA</t>
+          <t>NEW YORK</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CSCL YELLOW SEA</t>
+          <t>POLYNESIA</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CSYEL</t>
+          <t>PLYSA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0BHDQW1MA</t>
+          <t>0UAD1S1MA</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>COSCO SHIPPING LINES CO LTD</t>
+          <t>CMA - CGM</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>9645906</v>
+        <v>9477347</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>44868.95833333334</v>
+        <v>44880.875</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>44870.89583333334</v>
+        <v>44884.375</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>44870.95833333334</v>
+        <v>44884.5416666551</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>44875.0416666551</v>
+        <v>44885.375</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>USLAX</t>
+          <t>USNYC</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -882,29 +882,25 @@
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>TWPKS</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>LOS ANGELES, CA</t>
+          <t>NEW YORK</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CSCL SUMMER</t>
+          <t>COSCO FORTUNE</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>CSUMR</t>
+          <t>COFOR</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0TD9YW1MA</t>
+          <t>0MBCEW1MA</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -913,28 +909,28 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>9645865</v>
+        <v>9472127</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>44868.6875</v>
+        <v>44880.875</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>44869.64583333334</v>
+        <v>44876.3125</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>44869.6875</v>
+        <v>44880.45833333334</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>44870</v>
+        <v>44883.75555555556</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>USLAX</t>
+          <t>USNYC</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -949,52 +945,52 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>LONG BEACH, CA</t>
+          <t>NEW YORK</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DEBUSSY</t>
+          <t>EVER FASHION</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DBUSY</t>
+          <t>EVFSH</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0Y1BYS1MA</t>
+          <t>0VCD2W1MA</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ANL SINGAPORE PTE LTD</t>
+          <t>EVERGREEN MARINE CORPORATION LTD</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>9445576</v>
+        <v>9850836</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>44868.9375</v>
+        <v>44880.875</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>44870.25</v>
+        <v>44878.33333333334</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>44872.58333333334</v>
+        <v>44881.45833333334</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>44874.45833333334</v>
+        <v>44883.2916666551</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>USLGB</t>
+          <t>USNYC</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1009,52 +1005,52 @@
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>MIAMI</t>
+          <t>OAKLAND, CA</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CHICAGO EXPRESS</t>
+          <t>EVER LINKING</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>CHXPR</t>
+          <t>EVLKG</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0MRBOE1MA</t>
+          <t>0TBDGW1MA</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>HAPAG LLOYD</t>
+          <t>EVERGREEN MARINE CORPORATION LTD</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>9295268</v>
+        <v>9629043</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>44870.33333333334</v>
+        <v>44880.9166666551</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>44870.375</v>
+        <v>44881.0416666551</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>44871.7916666551</v>
+        <v>44883.08333333334</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>USMIA</t>
+          <t>USOAK</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1069,52 +1065,52 @@
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MIAMI</t>
+          <t>OAKLAND, CA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>VIENNA EXPRESS</t>
+          <t>CMA CGM NEW JERSEY</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>VNAXP</t>
+          <t>CGJEY</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0MRBSE1MA</t>
+          <t>0GVCDW1MA</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>HAPAG LLOYD</t>
+          <t>CMA - CGM</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>9450416</v>
+        <v>9351141</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>44868.875</v>
+        <v>44880</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>44873.35833333333</v>
+        <v>44881.9166666551</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>44873.44166665509</v>
+        <v>44882</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>44874.25</v>
+        <v>44883.5416666551</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>USMIA</t>
+          <t>USOAK</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1129,52 +1125,52 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MIAMI</t>
+          <t>NORFOLK</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AS SVENJA</t>
+          <t>MAERSK CHICAGO</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ASVEN</t>
+          <t>MKCHG</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0GY9CE1MA</t>
+          <t>1JU1ZE1MA</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>CMA - CGM</t>
+          <t>MSK</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>9410284</v>
+        <v>9332975</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880.875</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>44869.33333333334</v>
+        <v>44881.375</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>44869.4166666551</v>
+        <v>44881.5416666551</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>44869.875</v>
+        <v>44881.95833333334</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>USMIA</t>
+          <t>USORF</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1189,52 +1185,52 @@
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>MOBILE</t>
+          <t>SAVANNAH</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>COSCO ISTANBUL</t>
+          <t>CMA CGM LA TRAVIATA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CSISA</t>
+          <t>CMTRA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0TYD4W1MA</t>
+          <t>0MRBUE1MA</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>COSCO SHIPPING LINES CO LTD</t>
+          <t>CMA - CGM</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>9484340</v>
+        <v>9299795</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>44868.875</v>
+        <v>44880.875</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>44872.375</v>
+        <v>44881.69097222222</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>44872.5</v>
+        <v>44882.45833333334</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>44873.20833333334</v>
+        <v>44883.95833333334</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>USMOB</t>
+          <t>USSAV</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1249,22 +1245,22 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>MOBILE</t>
+          <t>SAVANNAH</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CMA CGM TANCREDI</t>
+          <t>CMA CGM APOLLON</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>CGTAN</t>
+          <t>CGAPO</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0PGDEW1MA</t>
+          <t>0MBC8W1MA</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1273,28 +1269,28 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>9436355</v>
+        <v>9882516</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>44868.9166666551</v>
+        <v>44880.83333333334</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>44873.75</v>
+        <v>44866.95833333334</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>44873.9166666551</v>
+        <v>44883.2916666551</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>44875</v>
+        <v>44885.95833333334</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>USMOB</t>
+          <t>USSAV</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1309,22 +1305,22 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NEW ORLEANS</t>
+          <t>SAVANNAH</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CMA CGM TANCREDI</t>
+          <t>SEATRADE BLUE</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>CGTAN</t>
+          <t>STBLE</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0PGDEW1MA</t>
+          <t>0RPBEN1MA</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1333,28 +1329,28 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>9436355</v>
+        <v>9756107</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>44868.9166666551</v>
+        <v>44880.875</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>44871.45833333334</v>
+        <v>44881.375</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>44871.95833333334</v>
+        <v>44881.5416666551</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>44872.7916666551</v>
+        <v>44882.1666666551</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>USMSY</t>
+          <t>USSAV</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1369,52 +1365,52 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>OAKLAND, CA</t>
+          <t>TACOMA, WA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>PRESIDENT CLEVELAND</t>
+          <t>EVER SUMMIT</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>PRCLE</t>
+          <t>EVSUM</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0DBDWW1MA</t>
+          <t>0NWD2W1MA</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>CMA CGM ASIA SHIPPING PTE. LTD</t>
+          <t>EVERGREEN MARINE CORPORATION LTD</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>9526502</v>
+        <v>9300453</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>44868.95833333334</v>
+        <v>44880</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>44868.25</v>
+        <v>44881.2916666551</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>44869.8541666551</v>
+        <v>44881.5416666551</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>44873.6666666551</v>
+        <v>44883.5416666551</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>USOAK</t>
+          <t>USTIW</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1429,52 +1425,52 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>NORFOLK</t>
+          <t>PORT EVERGLADES</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>VIENNA EXPRESS</t>
+          <t>POLAR CHILE</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>VNAXP</t>
+          <t>POCHL</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0MRBSE1MA</t>
+          <t>0AMCCN1MA</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>HAPAG LLOYD</t>
+          <t>MSK</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>9450416</v>
+        <v>9797187</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880.875</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>44870.83333333334</v>
+        <v>44886.6666666551</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>44870.95833333334</v>
+        <v>44886.75</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>44871.125</v>
+        <v>44887.125</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>USORF</t>
+          <t>USPEF</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1489,355 +1485,55 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PHILADELPHIA</t>
+          <t>PORT EVERGLADES</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>MATHILDE SCHULTE</t>
+          <t>NYK RUMINA</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>MATSH</t>
+          <t>NYRNA</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0RPBAN1MA</t>
+          <t>0CLCPW1MA</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>CMA - CGM</t>
+          <t>OCEAN NETWORK EXPRESS PTE. LTD.</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>9676709</v>
+        <v>9416991</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>44868.83333333334</v>
+        <v>44880.8541666551</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>44870.0416666551</v>
+        <v>44882.45833333334</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>44870.3541666551</v>
+        <v>44882.5</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>44870.875</v>
+        <v>44883.1666666551</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>USPHL</t>
+          <t>USPEF</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SAVANNAH</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>TOKYO TRIUMPH</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>TKYTR</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>0TSD0W1MA</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>EVERGREEN MARINE CORPORATION LTD</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>9737474</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>44868.83333333334</v>
-      </c>
-      <c r="K19" s="2" t="n">
-        <v>44859.75</v>
-      </c>
-      <c r="L19" s="2" t="n">
-        <v>44870.45833333334</v>
-      </c>
-      <c r="M19" s="2" t="n">
-        <v>44872.45833333334</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>2022-11-03</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>USSAV</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>SAVANNAH</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>MAERSK CHICAGO</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>MKCHG</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>1JU1ZE1MA</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>MSK</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>9332975</v>
-      </c>
-      <c r="J20" s="2" t="n">
-        <v>44868.83333333334</v>
-      </c>
-      <c r="K20" s="2" t="n">
-        <v>44870.33333333334</v>
-      </c>
-      <c r="L20" s="2" t="n">
-        <v>44870.5</v>
-      </c>
-      <c r="M20" s="2" t="n">
-        <v>44871.625</v>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>2022-11-03</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>USSAV</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>SAVANNAH</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>EVER FAITH</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>EVFAH</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>0VCCQW1MA</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>EVERGREEN MARINE CORPORATION LTD</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>9850525</v>
-      </c>
-      <c r="J21" s="2" t="n">
-        <v>44868.83333333334</v>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>44862.25</v>
-      </c>
-      <c r="L21" s="2" t="n">
-        <v>44870.83333333334</v>
-      </c>
-      <c r="M21" s="2" t="n">
-        <v>44871.83333333334</v>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>2022-11-03</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>USSAV</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>PORT EVERGLADES</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>CONTSHIP PAX</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>CSPAX</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>0AGAJS1MA</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>CMA - CGM</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>9435521</v>
-      </c>
-      <c r="J22" s="2" t="n">
-        <v>44868.83333333334</v>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>44869.30416665509</v>
-      </c>
-      <c r="L22" s="2" t="n">
-        <v>44869.4166666551</v>
-      </c>
-      <c r="M22" s="2" t="n">
-        <v>44870.4166666551</v>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>2022-11-03</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>USPEF</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>both</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>PORT EVERGLADES</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>NYK DELPHINUS</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>NYDPS</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>0CLCLW1MA</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>OCEAN NETWORK EXPRESS PTE. LTD.</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>9337652</v>
-      </c>
-      <c r="J23" s="2" t="n">
-        <v>44868.8125</v>
-      </c>
-      <c r="K23" s="2" t="n">
-        <v>44870.375</v>
-      </c>
-      <c r="L23" s="2" t="n">
-        <v>44870.4166666551</v>
-      </c>
-      <c r="M23" s="2" t="n">
-        <v>44870.8125</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>2022-11-03</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>USPEF</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
         <is>
           <t>both</t>
         </is>

</xml_diff>